<commit_message>
Added power meter readings
</commit_message>
<xml_diff>
--- a/rack_v2.0/PLC/type_A/data/global_variable_template.xlsx
+++ b/rack_v2.0/PLC/type_A/data/global_variable_template.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1554" uniqueCount="809">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1597" uniqueCount="837">
   <si>
     <t>[3(FALSE)]</t>
   </si>
@@ -1989,15 +1989,6 @@
     <t>1 - auto, 2- semiauto, 3 - manual</t>
   </si>
   <si>
-    <t>FEEDBACK_power_meter</t>
-  </si>
-  <si>
-    <t>D4450</t>
-  </si>
-  <si>
-    <t>Power reading</t>
-  </si>
-  <si>
     <t>CTRL_section_mode</t>
   </si>
   <si>
@@ -2464,6 +2455,99 @@
   </si>
   <si>
     <t>X1.11</t>
+  </si>
+  <si>
+    <t>MB_power_Ia</t>
+  </si>
+  <si>
+    <t>MB_power_Ib</t>
+  </si>
+  <si>
+    <t>MB_power_Ic</t>
+  </si>
+  <si>
+    <t>MB_power_kw</t>
+  </si>
+  <si>
+    <t>Power meter Kw total</t>
+  </si>
+  <si>
+    <t>Power meter Ia total</t>
+  </si>
+  <si>
+    <t>Power meter Ib total</t>
+  </si>
+  <si>
+    <t>Power meter Ic total</t>
+  </si>
+  <si>
+    <t>D25715</t>
+  </si>
+  <si>
+    <t>D25717</t>
+  </si>
+  <si>
+    <t>D25719</t>
+  </si>
+  <si>
+    <t>D25729</t>
+  </si>
+  <si>
+    <t>FEEDBACK_power_meter_KW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Power reading in KW </t>
+  </si>
+  <si>
+    <t>D4700</t>
+  </si>
+  <si>
+    <t>FEEDBACK_power_meter_Ia</t>
+  </si>
+  <si>
+    <t>FEEDBACK_power_meter_Ib</t>
+  </si>
+  <si>
+    <t>FEEDBACK_power_meter_Ic</t>
+  </si>
+  <si>
+    <t>D4705</t>
+  </si>
+  <si>
+    <t>D4710</t>
+  </si>
+  <si>
+    <t>D4715</t>
+  </si>
+  <si>
+    <t>Total Power reading in Ia</t>
+  </si>
+  <si>
+    <t>Total Power reading in Ib</t>
+  </si>
+  <si>
+    <t>Total Power reading in Ic</t>
+  </si>
+  <si>
+    <t>REF_pump_spin_limit</t>
+  </si>
+  <si>
+    <t>REF_pump_spin_limit_shutdown_time</t>
+  </si>
+  <si>
+    <t>Pump overspin limit</t>
+  </si>
+  <si>
+    <t>[3(10)]</t>
+  </si>
+  <si>
+    <t>Pump overspin limit time before shutdown</t>
+  </si>
+  <si>
+    <t>D4720</t>
+  </si>
+  <si>
+    <t>D4725</t>
   </si>
 </sst>
 </file>
@@ -2517,7 +2601,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2539,6 +2623,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3251,10 +3338,10 @@
         <v>12</v>
       </c>
       <c r="D24" t="s">
-        <v>792</v>
+        <v>789</v>
       </c>
       <c r="E24" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
       <c r="G24" t="s">
         <v>280</v>
@@ -3268,10 +3355,10 @@
         <v>12</v>
       </c>
       <c r="D25" t="s">
-        <v>792</v>
+        <v>789</v>
       </c>
       <c r="E25" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
       <c r="G25" t="s">
         <v>281</v>
@@ -3285,10 +3372,10 @@
         <v>12</v>
       </c>
       <c r="D26" t="s">
-        <v>792</v>
+        <v>789</v>
       </c>
       <c r="E26" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
       <c r="G26" t="s">
         <v>282</v>
@@ -3302,10 +3389,10 @@
         <v>12</v>
       </c>
       <c r="D27" t="s">
-        <v>792</v>
+        <v>789</v>
       </c>
       <c r="E27" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
       <c r="G27" t="s">
         <v>283</v>
@@ -3333,10 +3420,10 @@
         <v>12</v>
       </c>
       <c r="D29" t="s">
-        <v>793</v>
+        <v>790</v>
       </c>
       <c r="E29" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
       <c r="G29" t="s">
         <v>284</v>
@@ -3350,10 +3437,10 @@
         <v>12</v>
       </c>
       <c r="D30" t="s">
-        <v>793</v>
+        <v>790</v>
       </c>
       <c r="E30" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
       <c r="G30" t="s">
         <v>285</v>
@@ -3897,10 +3984,10 @@
         <v>12</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>793</v>
+        <v>790</v>
       </c>
       <c r="E59" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
       <c r="G59" t="s">
         <v>381</v>
@@ -3914,10 +4001,10 @@
         <v>12</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>793</v>
+        <v>790</v>
       </c>
       <c r="E60" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
       <c r="G60" t="s">
         <v>380</v>
@@ -3991,10 +4078,10 @@
         <v>12</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>794</v>
+        <v>791</v>
       </c>
       <c r="E64" t="s">
-        <v>795</v>
+        <v>792</v>
       </c>
       <c r="F64" t="s">
         <v>133</v>
@@ -4005,194 +4092,194 @@
     </row>
     <row r="65" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
       <c r="C65">
         <v>12</v>
       </c>
       <c r="D65" s="8" t="s">
-        <v>793</v>
+        <v>790</v>
       </c>
       <c r="E65" s="7" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
       <c r="G65" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
     </row>
     <row r="66" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>765</v>
+        <v>762</v>
       </c>
       <c r="C66">
         <v>12</v>
       </c>
       <c r="D66" s="8" t="s">
-        <v>793</v>
+        <v>790</v>
       </c>
       <c r="E66" s="7" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
       <c r="G66" t="s">
-        <v>691</v>
+        <v>688</v>
       </c>
     </row>
     <row r="67" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>766</v>
+        <v>763</v>
       </c>
       <c r="C67">
         <v>12</v>
       </c>
       <c r="D67" s="8" t="s">
-        <v>793</v>
+        <v>790</v>
       </c>
       <c r="E67" s="7" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
       <c r="G67" t="s">
-        <v>692</v>
+        <v>689</v>
       </c>
     </row>
     <row r="68" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>767</v>
+        <v>764</v>
       </c>
       <c r="C68">
         <v>12</v>
       </c>
       <c r="D68" s="8" t="s">
-        <v>793</v>
+        <v>790</v>
       </c>
       <c r="E68" s="7" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
       <c r="G68" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
     </row>
     <row r="69" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>768</v>
+        <v>765</v>
       </c>
       <c r="C69">
         <v>12</v>
       </c>
       <c r="D69" s="8" t="s">
-        <v>793</v>
+        <v>790</v>
       </c>
       <c r="E69" s="7" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
       <c r="G69" t="s">
-        <v>695</v>
+        <v>692</v>
       </c>
     </row>
     <row r="70" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>769</v>
+        <v>766</v>
       </c>
       <c r="C70">
         <v>12</v>
       </c>
       <c r="D70" s="8" t="s">
-        <v>793</v>
+        <v>790</v>
       </c>
       <c r="E70" s="7" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
       <c r="G70" t="s">
-        <v>697</v>
+        <v>694</v>
       </c>
     </row>
     <row r="71" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>770</v>
+        <v>767</v>
       </c>
       <c r="C71">
         <v>12</v>
       </c>
       <c r="D71" s="8" t="s">
-        <v>793</v>
+        <v>790</v>
       </c>
       <c r="E71" s="7" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
       <c r="G71" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
     </row>
     <row r="72" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="C72">
         <v>12</v>
       </c>
       <c r="D72" s="8" t="s">
-        <v>793</v>
+        <v>790</v>
       </c>
       <c r="E72" s="7" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
       <c r="G72" t="s">
-        <v>698</v>
+        <v>695</v>
       </c>
     </row>
     <row r="73" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
-        <v>772</v>
+        <v>769</v>
       </c>
       <c r="C73">
         <v>12</v>
       </c>
       <c r="D73" s="8" t="s">
-        <v>794</v>
+        <v>791</v>
       </c>
       <c r="E73" s="7" t="s">
-        <v>795</v>
+        <v>792</v>
       </c>
       <c r="G73" t="s">
-        <v>701</v>
+        <v>698</v>
       </c>
     </row>
     <row r="74" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
-        <v>785</v>
+        <v>782</v>
       </c>
       <c r="C74">
         <v>12</v>
       </c>
       <c r="D74" s="8" t="s">
-        <v>793</v>
+        <v>790</v>
       </c>
       <c r="E74" s="7" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
       <c r="G74" t="s">
-        <v>787</v>
+        <v>784</v>
       </c>
     </row>
     <row r="75" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
-        <v>786</v>
+        <v>783</v>
       </c>
       <c r="C75">
         <v>12</v>
       </c>
       <c r="D75" s="8" t="s">
-        <v>793</v>
+        <v>790</v>
       </c>
       <c r="E75" s="7" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
       <c r="G75" t="s">
-        <v>788</v>
+        <v>785</v>
       </c>
     </row>
     <row r="76" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
-        <v>789</v>
+        <v>786</v>
       </c>
       <c r="C76">
         <v>3</v>
@@ -4204,7 +4291,7 @@
         <v>0</v>
       </c>
       <c r="G76" t="s">
-        <v>790</v>
+        <v>787</v>
       </c>
     </row>
   </sheetData>
@@ -5952,10 +6039,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G190"/>
+  <dimension ref="A1:G199"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68"/>
+    <sheetView tabSelected="1" topLeftCell="A174" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K200" sqref="K200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5995,7 +6082,7 @@
         <v>476</v>
       </c>
       <c r="B2" t="s">
-        <v>752</v>
+        <v>749</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -6009,7 +6096,7 @@
         <v>477</v>
       </c>
       <c r="B3" t="s">
-        <v>721</v>
+        <v>718</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
@@ -6023,7 +6110,7 @@
         <v>478</v>
       </c>
       <c r="B4" t="s">
-        <v>722</v>
+        <v>719</v>
       </c>
       <c r="C4" t="s">
         <v>1</v>
@@ -6037,7 +6124,7 @@
         <v>479</v>
       </c>
       <c r="B5" t="s">
-        <v>723</v>
+        <v>720</v>
       </c>
       <c r="C5" t="s">
         <v>1</v>
@@ -6051,7 +6138,7 @@
         <v>480</v>
       </c>
       <c r="B6" t="s">
-        <v>753</v>
+        <v>750</v>
       </c>
       <c r="C6" t="s">
         <v>1</v>
@@ -6065,7 +6152,7 @@
         <v>481</v>
       </c>
       <c r="B7" t="s">
-        <v>724</v>
+        <v>721</v>
       </c>
       <c r="C7" t="s">
         <v>1</v>
@@ -6079,7 +6166,7 @@
         <v>482</v>
       </c>
       <c r="B8" t="s">
-        <v>725</v>
+        <v>722</v>
       </c>
       <c r="C8" t="s">
         <v>1</v>
@@ -6093,7 +6180,7 @@
         <v>483</v>
       </c>
       <c r="B9" t="s">
-        <v>726</v>
+        <v>723</v>
       </c>
       <c r="C9" t="s">
         <v>1</v>
@@ -6107,7 +6194,7 @@
         <v>484</v>
       </c>
       <c r="B10" t="s">
-        <v>754</v>
+        <v>751</v>
       </c>
       <c r="C10" t="s">
         <v>1</v>
@@ -6121,7 +6208,7 @@
         <v>485</v>
       </c>
       <c r="B11" t="s">
-        <v>727</v>
+        <v>724</v>
       </c>
       <c r="C11" t="s">
         <v>1</v>
@@ -6135,7 +6222,7 @@
         <v>486</v>
       </c>
       <c r="B12" t="s">
-        <v>728</v>
+        <v>725</v>
       </c>
       <c r="C12" t="s">
         <v>1</v>
@@ -6149,7 +6236,7 @@
         <v>487</v>
       </c>
       <c r="B13" t="s">
-        <v>729</v>
+        <v>726</v>
       </c>
       <c r="C13" t="s">
         <v>1</v>
@@ -6265,7 +6352,7 @@
         <v>494</v>
       </c>
       <c r="B20" t="s">
-        <v>705</v>
+        <v>702</v>
       </c>
       <c r="C20" t="s">
         <v>3</v>
@@ -6282,7 +6369,7 @@
         <v>495</v>
       </c>
       <c r="B21" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
       <c r="C21" t="s">
         <v>3</v>
@@ -6299,7 +6386,7 @@
         <v>496</v>
       </c>
       <c r="B22" t="s">
-        <v>707</v>
+        <v>704</v>
       </c>
       <c r="C22" t="s">
         <v>3</v>
@@ -6316,7 +6403,7 @@
         <v>497</v>
       </c>
       <c r="B23" t="s">
-        <v>708</v>
+        <v>705</v>
       </c>
       <c r="C23" t="s">
         <v>3</v>
@@ -6333,7 +6420,7 @@
         <v>498</v>
       </c>
       <c r="B24" t="s">
-        <v>709</v>
+        <v>706</v>
       </c>
       <c r="C24" t="s">
         <v>3</v>
@@ -6350,7 +6437,7 @@
         <v>499</v>
       </c>
       <c r="B25" t="s">
-        <v>710</v>
+        <v>707</v>
       </c>
       <c r="C25" t="s">
         <v>3</v>
@@ -6527,7 +6614,7 @@
         <v>411</v>
       </c>
       <c r="B34" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="C34" t="s">
         <v>3</v>
@@ -6539,7 +6626,7 @@
         <v>133</v>
       </c>
       <c r="F34" t="s">
-        <v>744</v>
+        <v>741</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -6547,7 +6634,7 @@
         <v>412</v>
       </c>
       <c r="B35" t="s">
-        <v>748</v>
+        <v>745</v>
       </c>
       <c r="C35" t="s">
         <v>3</v>
@@ -6559,7 +6646,7 @@
         <v>133</v>
       </c>
       <c r="F35" t="s">
-        <v>744</v>
+        <v>741</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -6856,7 +6943,7 @@
         <v>131</v>
       </c>
       <c r="F50" t="s">
-        <v>746</v>
+        <v>743</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -6873,7 +6960,7 @@
         <v>131</v>
       </c>
       <c r="F51" t="s">
-        <v>746</v>
+        <v>743</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -6890,7 +6977,7 @@
         <v>131</v>
       </c>
       <c r="F52" t="s">
-        <v>746</v>
+        <v>743</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -6907,12 +6994,12 @@
         <v>131</v>
       </c>
       <c r="F53" t="s">
-        <v>746</v>
+        <v>743</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>704</v>
+        <v>701</v>
       </c>
       <c r="B54" t="s">
         <v>466</v>
@@ -6924,12 +7011,12 @@
         <v>0</v>
       </c>
       <c r="F54" t="s">
-        <v>746</v>
+        <v>743</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>704</v>
+        <v>701</v>
       </c>
       <c r="B55" t="s">
         <v>467</v>
@@ -6941,7 +7028,7 @@
         <v>0</v>
       </c>
       <c r="F55" t="s">
-        <v>746</v>
+        <v>743</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -6958,7 +7045,7 @@
         <v>131</v>
       </c>
       <c r="F56" t="s">
-        <v>744</v>
+        <v>741</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
@@ -6975,7 +7062,7 @@
         <v>131</v>
       </c>
       <c r="F57" t="s">
-        <v>744</v>
+        <v>741</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -7119,7 +7206,7 @@
         <v>458</v>
       </c>
       <c r="B66" t="s">
-        <v>807</v>
+        <v>804</v>
       </c>
       <c r="C66" t="s">
         <v>3</v>
@@ -7136,7 +7223,7 @@
         <v>459</v>
       </c>
       <c r="B67" t="s">
-        <v>808</v>
+        <v>805</v>
       </c>
       <c r="C67" t="s">
         <v>3</v>
@@ -7153,7 +7240,7 @@
         <v>238</v>
       </c>
       <c r="B68" t="s">
-        <v>711</v>
+        <v>708</v>
       </c>
       <c r="C68" t="s">
         <v>3</v>
@@ -7170,7 +7257,7 @@
         <v>239</v>
       </c>
       <c r="B69" t="s">
-        <v>712</v>
+        <v>709</v>
       </c>
       <c r="C69" t="s">
         <v>3</v>
@@ -7187,7 +7274,7 @@
         <v>240</v>
       </c>
       <c r="B70" t="s">
-        <v>713</v>
+        <v>710</v>
       </c>
       <c r="C70" t="s">
         <v>3</v>
@@ -7204,7 +7291,7 @@
         <v>241</v>
       </c>
       <c r="B71" t="s">
-        <v>714</v>
+        <v>711</v>
       </c>
       <c r="C71" t="s">
         <v>3</v>
@@ -7221,7 +7308,7 @@
         <v>242</v>
       </c>
       <c r="B72" t="s">
-        <v>715</v>
+        <v>712</v>
       </c>
       <c r="C72" t="s">
         <v>3</v>
@@ -7238,7 +7325,7 @@
         <v>243</v>
       </c>
       <c r="B73" t="s">
-        <v>716</v>
+        <v>713</v>
       </c>
       <c r="C73" t="s">
         <v>3</v>
@@ -7255,7 +7342,7 @@
         <v>244</v>
       </c>
       <c r="B74" t="s">
-        <v>717</v>
+        <v>714</v>
       </c>
       <c r="C74" t="s">
         <v>3</v>
@@ -7272,7 +7359,7 @@
         <v>245</v>
       </c>
       <c r="B75" t="s">
-        <v>718</v>
+        <v>715</v>
       </c>
       <c r="C75" t="s">
         <v>3</v>
@@ -7289,7 +7376,7 @@
         <v>246</v>
       </c>
       <c r="B76" t="s">
-        <v>719</v>
+        <v>716</v>
       </c>
       <c r="C76" t="s">
         <v>3</v>
@@ -7306,7 +7393,7 @@
         <v>247</v>
       </c>
       <c r="B77" t="s">
-        <v>720</v>
+        <v>717</v>
       </c>
       <c r="C77" t="s">
         <v>3</v>
@@ -7323,7 +7410,7 @@
         <v>474</v>
       </c>
       <c r="B78" t="s">
-        <v>803</v>
+        <v>800</v>
       </c>
       <c r="C78" t="s">
         <v>3</v>
@@ -7340,7 +7427,7 @@
         <v>475</v>
       </c>
       <c r="B79" t="s">
-        <v>804</v>
+        <v>801</v>
       </c>
       <c r="C79" t="s">
         <v>3</v>
@@ -7357,7 +7444,7 @@
         <v>228</v>
       </c>
       <c r="B80" t="s">
-        <v>730</v>
+        <v>727</v>
       </c>
       <c r="C80" t="s">
         <v>1</v>
@@ -7366,7 +7453,7 @@
         <v>-1</v>
       </c>
       <c r="F80" t="s">
-        <v>745</v>
+        <v>742</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
@@ -7374,7 +7461,7 @@
         <v>229</v>
       </c>
       <c r="B81" t="s">
-        <v>731</v>
+        <v>728</v>
       </c>
       <c r="C81" t="s">
         <v>1</v>
@@ -7383,7 +7470,7 @@
         <v>-1</v>
       </c>
       <c r="F81" t="s">
-        <v>745</v>
+        <v>742</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
@@ -7391,7 +7478,7 @@
         <v>230</v>
       </c>
       <c r="B82" t="s">
-        <v>732</v>
+        <v>729</v>
       </c>
       <c r="C82" t="s">
         <v>1</v>
@@ -7408,7 +7495,7 @@
         <v>231</v>
       </c>
       <c r="B83" t="s">
-        <v>733</v>
+        <v>730</v>
       </c>
       <c r="C83" t="s">
         <v>1</v>
@@ -7425,7 +7512,7 @@
         <v>232</v>
       </c>
       <c r="B84" t="s">
-        <v>734</v>
+        <v>731</v>
       </c>
       <c r="C84" t="s">
         <v>1</v>
@@ -7442,7 +7529,7 @@
         <v>233</v>
       </c>
       <c r="B85" t="s">
-        <v>735</v>
+        <v>732</v>
       </c>
       <c r="C85" t="s">
         <v>1</v>
@@ -7459,7 +7546,7 @@
         <v>234</v>
       </c>
       <c r="B86" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
       <c r="C86" t="s">
         <v>1</v>
@@ -7476,7 +7563,7 @@
         <v>235</v>
       </c>
       <c r="B87" t="s">
-        <v>737</v>
+        <v>734</v>
       </c>
       <c r="C87" t="s">
         <v>1</v>
@@ -7493,7 +7580,7 @@
         <v>236</v>
       </c>
       <c r="B88" t="s">
-        <v>738</v>
+        <v>735</v>
       </c>
       <c r="C88" t="s">
         <v>1</v>
@@ -7510,7 +7597,7 @@
         <v>237</v>
       </c>
       <c r="B89" t="s">
-        <v>739</v>
+        <v>736</v>
       </c>
       <c r="C89" t="s">
         <v>1</v>
@@ -7527,7 +7614,7 @@
         <v>502</v>
       </c>
       <c r="B90" t="s">
-        <v>805</v>
+        <v>802</v>
       </c>
       <c r="C90" t="s">
         <v>1</v>
@@ -7544,7 +7631,7 @@
         <v>503</v>
       </c>
       <c r="B91" t="s">
-        <v>806</v>
+        <v>803</v>
       </c>
       <c r="C91" t="s">
         <v>1</v>
@@ -7561,7 +7648,7 @@
         <v>506</v>
       </c>
       <c r="B92" t="s">
-        <v>740</v>
+        <v>737</v>
       </c>
       <c r="C92" t="s">
         <v>1</v>
@@ -7578,7 +7665,7 @@
         <v>507</v>
       </c>
       <c r="B93" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="C93" t="s">
         <v>1</v>
@@ -7595,7 +7682,7 @@
         <v>508</v>
       </c>
       <c r="B94" t="s">
-        <v>742</v>
+        <v>739</v>
       </c>
       <c r="C94" t="s">
         <v>1</v>
@@ -7612,7 +7699,7 @@
         <v>509</v>
       </c>
       <c r="B95" t="s">
-        <v>743</v>
+        <v>740</v>
       </c>
       <c r="C95" t="s">
         <v>1</v>
@@ -8023,121 +8110,109 @@
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>317</v>
+        <v>806</v>
       </c>
       <c r="B119" t="s">
-        <v>315</v>
+        <v>814</v>
       </c>
       <c r="C119" t="s">
         <v>316</v>
       </c>
-      <c r="D119">
-        <v>0</v>
+      <c r="D119" s="10">
+        <v>-1</v>
+      </c>
+      <c r="F119" t="s">
+        <v>811</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>589</v>
+        <v>807</v>
       </c>
       <c r="B120" t="s">
-        <v>587</v>
+        <v>815</v>
       </c>
       <c r="C120" t="s">
-        <v>3</v>
-      </c>
-      <c r="D120">
-        <v>0</v>
+        <v>316</v>
+      </c>
+      <c r="D120" s="10">
+        <v>-1</v>
       </c>
       <c r="F120" t="s">
-        <v>588</v>
+        <v>812</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>584</v>
+        <v>808</v>
       </c>
       <c r="B121" t="s">
-        <v>585</v>
+        <v>816</v>
       </c>
       <c r="C121" t="s">
-        <v>1</v>
-      </c>
-      <c r="D121">
-        <v>0</v>
-      </c>
-      <c r="E121" t="s">
-        <v>133</v>
+        <v>316</v>
+      </c>
+      <c r="D121" s="10">
+        <v>-1</v>
       </c>
       <c r="F121" t="s">
-        <v>586</v>
+        <v>813</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>656</v>
+        <v>809</v>
       </c>
       <c r="B122" t="s">
-        <v>657</v>
+        <v>817</v>
       </c>
       <c r="C122" t="s">
-        <v>1</v>
-      </c>
-      <c r="D122">
-        <v>0</v>
-      </c>
-      <c r="E122" t="s">
-        <v>133</v>
+        <v>316</v>
+      </c>
+      <c r="D122" s="10">
+        <v>-1</v>
       </c>
       <c r="F122" t="s">
-        <v>660</v>
+        <v>810</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>658</v>
+        <v>317</v>
       </c>
       <c r="B123" t="s">
-        <v>659</v>
+        <v>315</v>
       </c>
       <c r="C123" t="s">
-        <v>1</v>
+        <v>316</v>
       </c>
       <c r="D123">
         <v>0</v>
       </c>
-      <c r="E123" t="s">
-        <v>133</v>
-      </c>
-      <c r="F123" t="s">
-        <v>660</v>
-      </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>661</v>
+        <v>589</v>
       </c>
       <c r="B124" t="s">
-        <v>662</v>
+        <v>587</v>
       </c>
       <c r="C124" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D124">
         <v>0</v>
       </c>
-      <c r="E124" t="s">
-        <v>133</v>
-      </c>
       <c r="F124" t="s">
-        <v>660</v>
+        <v>588</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>800</v>
+        <v>584</v>
       </c>
       <c r="B125" t="s">
-        <v>801</v>
+        <v>585</v>
       </c>
       <c r="C125" t="s">
         <v>1</v>
@@ -8149,38 +8224,38 @@
         <v>133</v>
       </c>
       <c r="F125" t="s">
-        <v>802</v>
+        <v>586</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>666</v>
+        <v>653</v>
       </c>
       <c r="B126" t="s">
-        <v>667</v>
+        <v>654</v>
       </c>
       <c r="C126" t="s">
-        <v>668</v>
-      </c>
-      <c r="D126" t="s">
-        <v>669</v>
+        <v>1</v>
+      </c>
+      <c r="D126">
+        <v>0</v>
       </c>
       <c r="E126" t="s">
         <v>133</v>
       </c>
       <c r="F126" t="s">
-        <v>670</v>
+        <v>657</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>749</v>
+        <v>655</v>
       </c>
       <c r="B127" t="s">
-        <v>750</v>
+        <v>656</v>
       </c>
       <c r="C127" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D127">
         <v>0</v>
@@ -8189,18 +8264,18 @@
         <v>133</v>
       </c>
       <c r="F127" t="s">
-        <v>751</v>
+        <v>657</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>761</v>
+        <v>658</v>
       </c>
       <c r="B128" t="s">
-        <v>762</v>
+        <v>659</v>
       </c>
       <c r="C128" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D128">
         <v>0</v>
@@ -8209,303 +8284,303 @@
         <v>133</v>
       </c>
       <c r="F128" t="s">
-        <v>763</v>
+        <v>657</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>607</v>
+        <v>797</v>
       </c>
       <c r="B129" t="s">
-        <v>332</v>
-      </c>
-      <c r="C129" s="8" t="s">
-        <v>793</v>
-      </c>
-      <c r="D129" t="s">
-        <v>791</v>
+        <v>798</v>
+      </c>
+      <c r="C129" t="s">
+        <v>1</v>
+      </c>
+      <c r="D129">
+        <v>0</v>
       </c>
       <c r="E129" t="s">
         <v>133</v>
       </c>
       <c r="F129" t="s">
-        <v>527</v>
+        <v>799</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>608</v>
+        <v>663</v>
       </c>
       <c r="B130" t="s">
-        <v>533</v>
-      </c>
-      <c r="C130" s="8" t="s">
-        <v>793</v>
+        <v>664</v>
+      </c>
+      <c r="C130" t="s">
+        <v>665</v>
       </c>
       <c r="D130" t="s">
-        <v>791</v>
+        <v>666</v>
       </c>
       <c r="E130" t="s">
         <v>133</v>
       </c>
       <c r="F130" t="s">
-        <v>528</v>
+        <v>667</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>609</v>
+        <v>746</v>
       </c>
       <c r="B131" t="s">
-        <v>534</v>
-      </c>
-      <c r="C131" s="8" t="s">
-        <v>793</v>
-      </c>
-      <c r="D131" t="s">
-        <v>791</v>
+        <v>747</v>
+      </c>
+      <c r="C131" t="s">
+        <v>3</v>
+      </c>
+      <c r="D131">
+        <v>0</v>
+      </c>
+      <c r="E131" t="s">
+        <v>133</v>
       </c>
       <c r="F131" t="s">
-        <v>540</v>
+        <v>748</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>600</v>
+        <v>758</v>
       </c>
       <c r="B132" t="s">
-        <v>604</v>
-      </c>
-      <c r="C132" s="8" t="s">
-        <v>601</v>
-      </c>
-      <c r="D132" t="s">
-        <v>602</v>
+        <v>759</v>
+      </c>
+      <c r="C132" t="s">
+        <v>3</v>
+      </c>
+      <c r="D132">
+        <v>0</v>
+      </c>
+      <c r="E132" t="s">
+        <v>133</v>
       </c>
       <c r="F132" t="s">
-        <v>603</v>
+        <v>760</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>524</v>
+        <v>607</v>
       </c>
       <c r="B133" t="s">
-        <v>539</v>
+        <v>332</v>
       </c>
       <c r="C133" s="8" t="s">
-        <v>793</v>
+        <v>790</v>
       </c>
       <c r="D133" t="s">
-        <v>791</v>
+        <v>788</v>
+      </c>
+      <c r="E133" t="s">
+        <v>133</v>
       </c>
       <c r="F133" t="s">
-        <v>545</v>
+        <v>527</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>541</v>
+        <v>608</v>
       </c>
       <c r="B134" t="s">
-        <v>542</v>
-      </c>
-      <c r="C134" t="s">
-        <v>794</v>
+        <v>533</v>
+      </c>
+      <c r="C134" s="8" t="s">
+        <v>790</v>
       </c>
       <c r="D134" t="s">
-        <v>795</v>
+        <v>788</v>
+      </c>
+      <c r="E134" t="s">
+        <v>133</v>
       </c>
       <c r="F134" t="s">
-        <v>543</v>
+        <v>528</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>776</v>
+        <v>609</v>
       </c>
       <c r="B135" t="s">
-        <v>777</v>
+        <v>534</v>
       </c>
       <c r="C135" s="8" t="s">
-        <v>793</v>
+        <v>790</v>
       </c>
       <c r="D135" t="s">
-        <v>791</v>
-      </c>
-      <c r="E135" t="s">
-        <v>133</v>
+        <v>788</v>
       </c>
       <c r="F135" t="s">
-        <v>778</v>
+        <v>540</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>605</v>
+        <v>600</v>
       </c>
       <c r="B136" t="s">
-        <v>535</v>
-      </c>
-      <c r="C136" t="s">
-        <v>2</v>
+        <v>604</v>
+      </c>
+      <c r="C136" s="8" t="s">
+        <v>601</v>
       </c>
       <c r="D136" t="s">
-        <v>0</v>
-      </c>
-      <c r="E136" t="s">
-        <v>133</v>
+        <v>602</v>
       </c>
       <c r="F136" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>529</v>
+        <v>524</v>
       </c>
       <c r="B137" t="s">
-        <v>536</v>
+        <v>539</v>
       </c>
       <c r="C137" s="8" t="s">
-        <v>11</v>
+        <v>790</v>
       </c>
       <c r="D137" t="s">
-        <v>12</v>
-      </c>
-      <c r="E137" t="s">
-        <v>133</v>
+        <v>788</v>
       </c>
       <c r="F137" t="s">
-        <v>530</v>
+        <v>545</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>531</v>
+        <v>541</v>
       </c>
       <c r="B138" t="s">
-        <v>537</v>
-      </c>
-      <c r="C138" s="8" t="s">
-        <v>11</v>
+        <v>542</v>
+      </c>
+      <c r="C138" t="s">
+        <v>791</v>
       </c>
       <c r="D138" t="s">
-        <v>12</v>
-      </c>
-      <c r="E138" t="s">
-        <v>133</v>
+        <v>792</v>
       </c>
       <c r="F138" t="s">
-        <v>532</v>
+        <v>543</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>546</v>
+        <v>773</v>
       </c>
       <c r="B139" t="s">
-        <v>548</v>
+        <v>774</v>
       </c>
       <c r="C139" s="8" t="s">
-        <v>11</v>
+        <v>790</v>
       </c>
       <c r="D139" t="s">
-        <v>12</v>
+        <v>788</v>
       </c>
       <c r="E139" t="s">
         <v>133</v>
       </c>
       <c r="F139" t="s">
-        <v>550</v>
+        <v>775</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>547</v>
+        <v>605</v>
       </c>
       <c r="B140" t="s">
-        <v>538</v>
-      </c>
-      <c r="C140" s="8" t="s">
-        <v>11</v>
+        <v>535</v>
+      </c>
+      <c r="C140" t="s">
+        <v>2</v>
       </c>
       <c r="D140" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="E140" t="s">
         <v>133</v>
       </c>
       <c r="F140" t="s">
-        <v>551</v>
+        <v>606</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>674</v>
+        <v>529</v>
       </c>
       <c r="B141" t="s">
-        <v>675</v>
-      </c>
-      <c r="C141" t="s">
-        <v>2</v>
+        <v>536</v>
+      </c>
+      <c r="C141" s="8" t="s">
+        <v>11</v>
       </c>
       <c r="D141" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="E141" t="s">
         <v>133</v>
       </c>
       <c r="F141" t="s">
-        <v>676</v>
+        <v>530</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>552</v>
+        <v>531</v>
       </c>
       <c r="B142" t="s">
-        <v>549</v>
-      </c>
-      <c r="C142" t="s">
-        <v>2</v>
+        <v>537</v>
+      </c>
+      <c r="C142" s="8" t="s">
+        <v>11</v>
       </c>
       <c r="D142" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="E142" t="s">
         <v>133</v>
       </c>
       <c r="F142" t="s">
-        <v>553</v>
+        <v>532</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>554</v>
+        <v>546</v>
       </c>
       <c r="B143" t="s">
-        <v>556</v>
-      </c>
-      <c r="C143" t="s">
-        <v>2</v>
+        <v>548</v>
+      </c>
+      <c r="C143" s="8" t="s">
+        <v>11</v>
       </c>
       <c r="D143" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="E143" t="s">
         <v>133</v>
       </c>
       <c r="F143" t="s">
-        <v>558</v>
+        <v>550</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>673</v>
+        <v>547</v>
       </c>
       <c r="B144" t="s">
-        <v>671</v>
+        <v>538</v>
       </c>
       <c r="C144" s="8" t="s">
         <v>11</v>
@@ -8517,69 +8592,75 @@
         <v>133</v>
       </c>
       <c r="F144" t="s">
-        <v>672</v>
+        <v>551</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>525</v>
+        <v>671</v>
       </c>
       <c r="B145" t="s">
-        <v>555</v>
+        <v>672</v>
       </c>
       <c r="C145" t="s">
-        <v>794</v>
+        <v>2</v>
       </c>
       <c r="D145" t="s">
-        <v>795</v>
+        <v>0</v>
+      </c>
+      <c r="E145" t="s">
+        <v>133</v>
       </c>
       <c r="F145" t="s">
-        <v>560</v>
+        <v>673</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>526</v>
+        <v>552</v>
       </c>
       <c r="B146" t="s">
-        <v>557</v>
-      </c>
-      <c r="C146" s="8" t="s">
-        <v>793</v>
+        <v>549</v>
+      </c>
+      <c r="C146" t="s">
+        <v>2</v>
       </c>
       <c r="D146" t="s">
-        <v>791</v>
+        <v>0</v>
+      </c>
+      <c r="E146" t="s">
+        <v>133</v>
       </c>
       <c r="F146" t="s">
-        <v>544</v>
+        <v>553</v>
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>564</v>
+        <v>554</v>
       </c>
       <c r="B147" t="s">
-        <v>567</v>
-      </c>
-      <c r="C147" s="8" t="s">
-        <v>11</v>
+        <v>556</v>
+      </c>
+      <c r="C147" t="s">
+        <v>2</v>
       </c>
       <c r="D147" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="E147" t="s">
         <v>133</v>
       </c>
       <c r="F147" t="s">
-        <v>610</v>
+        <v>558</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>565</v>
+        <v>670</v>
       </c>
       <c r="B148" t="s">
-        <v>570</v>
+        <v>668</v>
       </c>
       <c r="C148" s="8" t="s">
         <v>11</v>
@@ -8591,401 +8672,407 @@
         <v>133</v>
       </c>
       <c r="F148" t="s">
-        <v>568</v>
+        <v>669</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>566</v>
+        <v>525</v>
       </c>
       <c r="B149" t="s">
-        <v>571</v>
-      </c>
-      <c r="C149" s="8" t="s">
-        <v>11</v>
+        <v>555</v>
+      </c>
+      <c r="C149" t="s">
+        <v>791</v>
       </c>
       <c r="D149" t="s">
-        <v>12</v>
-      </c>
-      <c r="E149" t="s">
-        <v>133</v>
+        <v>792</v>
       </c>
       <c r="F149" t="s">
-        <v>569</v>
+        <v>560</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>559</v>
+        <v>526</v>
       </c>
       <c r="B150" t="s">
-        <v>572</v>
-      </c>
-      <c r="C150" t="s">
-        <v>2</v>
+        <v>557</v>
+      </c>
+      <c r="C150" s="8" t="s">
+        <v>790</v>
       </c>
       <c r="D150" t="s">
-        <v>0</v>
+        <v>788</v>
       </c>
       <c r="F150" t="s">
-        <v>562</v>
+        <v>544</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>561</v>
+        <v>564</v>
       </c>
       <c r="B151" t="s">
-        <v>574</v>
-      </c>
-      <c r="C151" t="s">
-        <v>2</v>
+        <v>567</v>
+      </c>
+      <c r="C151" s="8" t="s">
+        <v>11</v>
       </c>
       <c r="D151" t="s">
-        <v>0</v>
+        <v>12</v>
+      </c>
+      <c r="E151" t="s">
+        <v>133</v>
       </c>
       <c r="F151" t="s">
-        <v>563</v>
+        <v>610</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>575</v>
+        <v>565</v>
       </c>
       <c r="B152" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="C152" s="8" t="s">
-        <v>793</v>
+        <v>11</v>
       </c>
       <c r="D152" t="s">
-        <v>791</v>
+        <v>12</v>
+      </c>
+      <c r="E152" t="s">
+        <v>133</v>
       </c>
       <c r="F152" t="s">
-        <v>212</v>
+        <v>568</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>576</v>
+        <v>566</v>
       </c>
       <c r="B153" t="s">
-        <v>621</v>
+        <v>571</v>
       </c>
       <c r="C153" s="8" t="s">
-        <v>793</v>
+        <v>11</v>
       </c>
       <c r="D153" t="s">
-        <v>791</v>
+        <v>12</v>
+      </c>
+      <c r="E153" t="s">
+        <v>133</v>
       </c>
       <c r="F153" t="s">
-        <v>211</v>
+        <v>569</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>577</v>
+        <v>559</v>
       </c>
       <c r="B154" t="s">
-        <v>622</v>
-      </c>
-      <c r="C154" s="8" t="s">
-        <v>793</v>
+        <v>572</v>
+      </c>
+      <c r="C154" t="s">
+        <v>2</v>
       </c>
       <c r="D154" t="s">
-        <v>791</v>
+        <v>0</v>
       </c>
       <c r="F154" t="s">
-        <v>213</v>
+        <v>562</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>578</v>
+        <v>561</v>
       </c>
       <c r="B155" t="s">
-        <v>623</v>
-      </c>
-      <c r="C155" s="8" t="s">
-        <v>793</v>
+        <v>574</v>
+      </c>
+      <c r="C155" t="s">
+        <v>2</v>
       </c>
       <c r="D155" t="s">
-        <v>791</v>
+        <v>0</v>
       </c>
       <c r="F155" t="s">
-        <v>214</v>
+        <v>563</v>
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="B156" t="s">
-        <v>624</v>
+        <v>573</v>
       </c>
       <c r="C156" s="8" t="s">
-        <v>793</v>
+        <v>790</v>
       </c>
       <c r="D156" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
       <c r="F156" t="s">
-        <v>522</v>
+        <v>212</v>
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
       <c r="B157" t="s">
-        <v>626</v>
+        <v>621</v>
       </c>
       <c r="C157" s="8" t="s">
-        <v>793</v>
+        <v>790</v>
       </c>
       <c r="D157" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
       <c r="F157" t="s">
-        <v>523</v>
+        <v>211</v>
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>615</v>
+        <v>577</v>
       </c>
       <c r="B158" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
       <c r="C158" s="8" t="s">
-        <v>793</v>
+        <v>790</v>
       </c>
       <c r="D158" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
       <c r="F158" t="s">
-        <v>632</v>
+        <v>213</v>
       </c>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>616</v>
+        <v>578</v>
       </c>
       <c r="B159" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
       <c r="C159" s="8" t="s">
-        <v>793</v>
+        <v>790</v>
       </c>
       <c r="D159" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
       <c r="F159" t="s">
-        <v>633</v>
+        <v>214</v>
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>617</v>
+        <v>579</v>
       </c>
       <c r="B160" t="s">
-        <v>628</v>
+        <v>624</v>
       </c>
       <c r="C160" s="8" t="s">
-        <v>793</v>
+        <v>790</v>
       </c>
       <c r="D160" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
       <c r="F160" t="s">
-        <v>634</v>
+        <v>522</v>
       </c>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>618</v>
+        <v>580</v>
       </c>
       <c r="B161" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="C161" s="8" t="s">
-        <v>793</v>
+        <v>790</v>
       </c>
       <c r="D161" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
       <c r="F161" t="s">
-        <v>635</v>
+        <v>523</v>
       </c>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>619</v>
+        <v>615</v>
       </c>
       <c r="B162" t="s">
-        <v>630</v>
+        <v>625</v>
       </c>
       <c r="C162" s="8" t="s">
-        <v>793</v>
+        <v>790</v>
       </c>
       <c r="D162" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
       <c r="F162" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
       <c r="B163" t="s">
-        <v>631</v>
+        <v>627</v>
       </c>
       <c r="C163" s="8" t="s">
-        <v>793</v>
+        <v>790</v>
       </c>
       <c r="D163" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
       <c r="F163" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>581</v>
+        <v>617</v>
       </c>
       <c r="B164" t="s">
-        <v>638</v>
+        <v>628</v>
       </c>
       <c r="C164" s="8" t="s">
-        <v>793</v>
+        <v>790</v>
       </c>
       <c r="D164" t="s">
-        <v>791</v>
-      </c>
-      <c r="E164" t="s">
-        <v>133</v>
+        <v>788</v>
       </c>
       <c r="F164" t="s">
-        <v>215</v>
+        <v>634</v>
       </c>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>582</v>
+        <v>618</v>
       </c>
       <c r="B165" t="s">
-        <v>639</v>
+        <v>629</v>
       </c>
       <c r="C165" s="8" t="s">
-        <v>793</v>
+        <v>790</v>
       </c>
       <c r="D165" t="s">
-        <v>791</v>
-      </c>
-      <c r="E165" t="s">
-        <v>133</v>
+        <v>788</v>
       </c>
       <c r="F165" t="s">
-        <v>216</v>
+        <v>635</v>
       </c>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>583</v>
+        <v>619</v>
       </c>
       <c r="B166" t="s">
-        <v>640</v>
+        <v>630</v>
       </c>
       <c r="C166" s="8" t="s">
-        <v>793</v>
+        <v>790</v>
       </c>
       <c r="D166" t="s">
-        <v>791</v>
-      </c>
-      <c r="E166" t="s">
-        <v>133</v>
+        <v>788</v>
       </c>
       <c r="F166" t="s">
-        <v>217</v>
+        <v>636</v>
       </c>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>590</v>
+        <v>620</v>
       </c>
       <c r="B167" t="s">
-        <v>641</v>
+        <v>631</v>
       </c>
       <c r="C167" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D167" s="7" t="s">
-        <v>12</v>
+        <v>790</v>
+      </c>
+      <c r="D167" t="s">
+        <v>788</v>
       </c>
       <c r="F167" t="s">
-        <v>592</v>
+        <v>637</v>
       </c>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>591</v>
+        <v>581</v>
       </c>
       <c r="B168" t="s">
-        <v>642</v>
+        <v>638</v>
       </c>
       <c r="C168" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D168" s="7" t="s">
-        <v>12</v>
+        <v>790</v>
+      </c>
+      <c r="D168" t="s">
+        <v>788</v>
+      </c>
+      <c r="E168" t="s">
+        <v>133</v>
       </c>
       <c r="F168" t="s">
-        <v>593</v>
+        <v>215</v>
       </c>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>595</v>
+        <v>582</v>
       </c>
       <c r="B169" t="s">
-        <v>643</v>
+        <v>639</v>
       </c>
       <c r="C169" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D169" s="7" t="s">
-        <v>12</v>
+        <v>790</v>
+      </c>
+      <c r="D169" t="s">
+        <v>788</v>
+      </c>
+      <c r="E169" t="s">
+        <v>133</v>
       </c>
       <c r="F169" t="s">
-        <v>594</v>
+        <v>216</v>
       </c>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>597</v>
+        <v>583</v>
       </c>
       <c r="B170" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
       <c r="C170" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D170" s="7" t="s">
-        <v>0</v>
+        <v>790</v>
+      </c>
+      <c r="D170" t="s">
+        <v>788</v>
+      </c>
+      <c r="E170" t="s">
+        <v>133</v>
       </c>
       <c r="F170" t="s">
-        <v>596</v>
+        <v>217</v>
       </c>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>598</v>
+        <v>590</v>
       </c>
       <c r="B171" t="s">
-        <v>645</v>
+        <v>641</v>
       </c>
       <c r="C171" s="8" t="s">
         <v>11</v>
@@ -8994,75 +9081,66 @@
         <v>12</v>
       </c>
       <c r="F171" t="s">
-        <v>599</v>
+        <v>592</v>
       </c>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>611</v>
+        <v>591</v>
       </c>
       <c r="B172" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
       <c r="C172" s="8" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="D172" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E172" t="s">
-        <v>133</v>
+        <v>12</v>
       </c>
       <c r="F172" t="s">
-        <v>612</v>
+        <v>593</v>
       </c>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>613</v>
+        <v>595</v>
       </c>
       <c r="B173" t="s">
-        <v>647</v>
+        <v>643</v>
       </c>
       <c r="C173" s="8" t="s">
-        <v>796</v>
+        <v>11</v>
       </c>
       <c r="D173" s="7" t="s">
-        <v>797</v>
-      </c>
-      <c r="E173" t="s">
-        <v>133</v>
+        <v>12</v>
       </c>
       <c r="F173" t="s">
-        <v>614</v>
+        <v>594</v>
       </c>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>650</v>
+        <v>597</v>
       </c>
       <c r="B174" t="s">
-        <v>651</v>
+        <v>644</v>
       </c>
       <c r="C174" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="D174">
+        <v>2</v>
+      </c>
+      <c r="D174" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="E174" t="s">
-        <v>133</v>
-      </c>
       <c r="F174" t="s">
-        <v>652</v>
+        <v>596</v>
       </c>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>653</v>
+        <v>598</v>
       </c>
       <c r="B175" t="s">
-        <v>654</v>
+        <v>645</v>
       </c>
       <c r="C175" s="8" t="s">
         <v>11</v>
@@ -9070,311 +9148,488 @@
       <c r="D175" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E175" t="s">
-        <v>133</v>
-      </c>
       <c r="F175" t="s">
-        <v>655</v>
+        <v>599</v>
       </c>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>663</v>
+        <v>611</v>
       </c>
       <c r="B176" t="s">
-        <v>664</v>
+        <v>646</v>
       </c>
       <c r="C176" s="8" t="s">
-        <v>794</v>
+        <v>2</v>
       </c>
       <c r="D176" s="7" t="s">
-        <v>795</v>
+        <v>0</v>
       </c>
       <c r="E176" t="s">
         <v>133</v>
       </c>
       <c r="F176" t="s">
-        <v>665</v>
+        <v>612</v>
       </c>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>678</v>
+        <v>613</v>
       </c>
       <c r="B177" t="s">
-        <v>677</v>
+        <v>647</v>
       </c>
       <c r="C177" s="8" t="s">
         <v>793</v>
       </c>
-      <c r="D177" t="s">
-        <v>791</v>
+      <c r="D177" s="7" t="s">
+        <v>794</v>
       </c>
       <c r="E177" t="s">
         <v>133</v>
       </c>
       <c r="F177" t="s">
-        <v>694</v>
+        <v>614</v>
       </c>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>679</v>
+        <v>650</v>
       </c>
       <c r="B178" t="s">
-        <v>686</v>
+        <v>651</v>
       </c>
       <c r="C178" s="8" t="s">
-        <v>793</v>
-      </c>
-      <c r="D178" t="s">
-        <v>791</v>
+        <v>11</v>
+      </c>
+      <c r="D178" s="7" t="s">
+        <v>12</v>
       </c>
       <c r="E178" t="s">
         <v>133</v>
       </c>
       <c r="F178" t="s">
-        <v>691</v>
+        <v>652</v>
       </c>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>680</v>
+        <v>660</v>
       </c>
       <c r="B179" t="s">
-        <v>687</v>
+        <v>661</v>
       </c>
       <c r="C179" s="8" t="s">
-        <v>793</v>
-      </c>
-      <c r="D179" t="s">
         <v>791</v>
       </c>
+      <c r="D179" s="7" t="s">
+        <v>792</v>
+      </c>
       <c r="E179" t="s">
         <v>133</v>
       </c>
       <c r="F179" t="s">
-        <v>692</v>
+        <v>662</v>
       </c>
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>681</v>
+        <v>675</v>
       </c>
       <c r="B180" t="s">
-        <v>688</v>
+        <v>674</v>
       </c>
       <c r="C180" s="8" t="s">
-        <v>793</v>
+        <v>790</v>
       </c>
       <c r="D180" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
       <c r="E180" t="s">
         <v>133</v>
       </c>
       <c r="F180" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>682</v>
+        <v>676</v>
       </c>
       <c r="B181" t="s">
-        <v>689</v>
+        <v>683</v>
       </c>
       <c r="C181" s="8" t="s">
-        <v>793</v>
+        <v>790</v>
       </c>
       <c r="D181" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
       <c r="E181" t="s">
         <v>133</v>
       </c>
       <c r="F181" t="s">
-        <v>695</v>
+        <v>688</v>
       </c>
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>683</v>
+        <v>677</v>
       </c>
       <c r="B182" t="s">
-        <v>690</v>
+        <v>684</v>
       </c>
       <c r="C182" s="8" t="s">
-        <v>793</v>
+        <v>790</v>
       </c>
       <c r="D182" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
       <c r="E182" t="s">
         <v>133</v>
       </c>
       <c r="F182" t="s">
-        <v>697</v>
+        <v>689</v>
       </c>
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>684</v>
+        <v>678</v>
       </c>
       <c r="B183" t="s">
-        <v>699</v>
+        <v>685</v>
       </c>
       <c r="C183" s="8" t="s">
-        <v>793</v>
+        <v>790</v>
       </c>
       <c r="D183" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
       <c r="E183" t="s">
         <v>133</v>
       </c>
       <c r="F183" t="s">
-        <v>696</v>
+        <v>690</v>
       </c>
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>685</v>
+        <v>679</v>
       </c>
       <c r="B184" t="s">
-        <v>700</v>
+        <v>686</v>
       </c>
       <c r="C184" s="8" t="s">
-        <v>793</v>
+        <v>790</v>
       </c>
       <c r="D184" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
       <c r="E184" t="s">
         <v>133</v>
       </c>
       <c r="F184" t="s">
-        <v>698</v>
+        <v>692</v>
       </c>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>702</v>
+        <v>680</v>
       </c>
       <c r="B185" t="s">
-        <v>703</v>
+        <v>687</v>
       </c>
       <c r="C185" s="8" t="s">
-        <v>794</v>
-      </c>
-      <c r="D185" s="7" t="s">
-        <v>795</v>
+        <v>790</v>
+      </c>
+      <c r="D185" t="s">
+        <v>788</v>
       </c>
       <c r="E185" t="s">
         <v>133</v>
       </c>
       <c r="F185" t="s">
-        <v>701</v>
+        <v>694</v>
       </c>
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>755</v>
+        <v>681</v>
       </c>
       <c r="B186" t="s">
-        <v>756</v>
+        <v>696</v>
       </c>
       <c r="C186" s="8" t="s">
-        <v>514</v>
-      </c>
-      <c r="D186" s="7" t="s">
-        <v>515</v>
+        <v>790</v>
+      </c>
+      <c r="D186" t="s">
+        <v>788</v>
       </c>
       <c r="E186" t="s">
         <v>133</v>
       </c>
       <c r="F186" t="s">
-        <v>757</v>
+        <v>693</v>
       </c>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>758</v>
+        <v>682</v>
       </c>
       <c r="B187" t="s">
-        <v>759</v>
+        <v>697</v>
       </c>
       <c r="C187" s="8" t="s">
-        <v>793</v>
-      </c>
-      <c r="D187" s="7" t="s">
-        <v>791</v>
+        <v>790</v>
+      </c>
+      <c r="D187" t="s">
+        <v>788</v>
       </c>
       <c r="E187" t="s">
         <v>133</v>
       </c>
       <c r="F187" t="s">
-        <v>760</v>
+        <v>695</v>
       </c>
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>773</v>
+        <v>699</v>
       </c>
       <c r="B188" t="s">
-        <v>774</v>
+        <v>700</v>
       </c>
       <c r="C188" s="8" t="s">
-        <v>2</v>
+        <v>791</v>
       </c>
       <c r="D188" s="7" t="s">
-        <v>0</v>
+        <v>792</v>
       </c>
       <c r="E188" t="s">
         <v>133</v>
       </c>
       <c r="F188" t="s">
-        <v>775</v>
+        <v>698</v>
       </c>
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>779</v>
+        <v>752</v>
       </c>
       <c r="B189" t="s">
-        <v>780</v>
+        <v>753</v>
       </c>
       <c r="C189" s="8" t="s">
-        <v>793</v>
-      </c>
-      <c r="D189" t="s">
-        <v>791</v>
+        <v>514</v>
+      </c>
+      <c r="D189" s="7" t="s">
+        <v>515</v>
       </c>
       <c r="E189" t="s">
         <v>133</v>
       </c>
       <c r="F189" t="s">
-        <v>783</v>
+        <v>754</v>
       </c>
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
+        <v>755</v>
+      </c>
+      <c r="B190" t="s">
+        <v>756</v>
+      </c>
+      <c r="C190" s="8" t="s">
+        <v>790</v>
+      </c>
+      <c r="D190" s="7" t="s">
+        <v>788</v>
+      </c>
+      <c r="E190" t="s">
+        <v>133</v>
+      </c>
+      <c r="F190" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
+        <v>770</v>
+      </c>
+      <c r="B191" t="s">
+        <v>771</v>
+      </c>
+      <c r="C191" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D191" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E191" t="s">
+        <v>133</v>
+      </c>
+      <c r="F191" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
+        <v>776</v>
+      </c>
+      <c r="B192" t="s">
+        <v>777</v>
+      </c>
+      <c r="C192" s="8" t="s">
+        <v>790</v>
+      </c>
+      <c r="D192" t="s">
+        <v>788</v>
+      </c>
+      <c r="E192" t="s">
+        <v>133</v>
+      </c>
+      <c r="F192" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
+        <v>778</v>
+      </c>
+      <c r="B193" t="s">
+        <v>779</v>
+      </c>
+      <c r="C193" s="8" t="s">
+        <v>790</v>
+      </c>
+      <c r="D193" t="s">
+        <v>788</v>
+      </c>
+      <c r="E193" t="s">
+        <v>133</v>
+      </c>
+      <c r="F193" t="s">
         <v>781</v>
       </c>
-      <c r="B190" t="s">
-        <v>782</v>
-      </c>
-      <c r="C190" s="8" t="s">
-        <v>793</v>
-      </c>
-      <c r="D190" t="s">
-        <v>791</v>
-      </c>
-      <c r="E190" t="s">
-        <v>133</v>
-      </c>
-      <c r="F190" t="s">
-        <v>784</v>
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
+        <v>830</v>
+      </c>
+      <c r="B194" t="s">
+        <v>820</v>
+      </c>
+      <c r="C194" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D194" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E194" t="s">
+        <v>133</v>
+      </c>
+      <c r="F194" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
+        <v>831</v>
+      </c>
+      <c r="B195" t="s">
+        <v>824</v>
+      </c>
+      <c r="C195" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D195" s="7" t="s">
+        <v>833</v>
+      </c>
+      <c r="E195" t="s">
+        <v>133</v>
+      </c>
+      <c r="F195" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
+        <v>818</v>
+      </c>
+      <c r="B196" t="s">
+        <v>825</v>
+      </c>
+      <c r="C196" s="8" t="s">
+        <v>316</v>
+      </c>
+      <c r="D196">
+        <v>0</v>
+      </c>
+      <c r="E196" t="s">
+        <v>133</v>
+      </c>
+      <c r="F196" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
+        <v>821</v>
+      </c>
+      <c r="B197" t="s">
+        <v>826</v>
+      </c>
+      <c r="C197" s="8" t="s">
+        <v>316</v>
+      </c>
+      <c r="D197">
+        <v>0</v>
+      </c>
+      <c r="E197" t="s">
+        <v>133</v>
+      </c>
+      <c r="F197" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
+        <v>822</v>
+      </c>
+      <c r="B198" t="s">
+        <v>835</v>
+      </c>
+      <c r="C198" s="8" t="s">
+        <v>316</v>
+      </c>
+      <c r="D198">
+        <v>0</v>
+      </c>
+      <c r="E198" t="s">
+        <v>133</v>
+      </c>
+      <c r="F198" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
+        <v>823</v>
+      </c>
+      <c r="B199" t="s">
+        <v>836</v>
+      </c>
+      <c r="C199" s="8" t="s">
+        <v>316</v>
+      </c>
+      <c r="D199">
+        <v>0</v>
+      </c>
+      <c r="E199" t="s">
+        <v>133</v>
+      </c>
+      <c r="F199" t="s">
+        <v>829</v>
       </c>
     </row>
   </sheetData>
@@ -9424,10 +9679,10 @@
         <v>1000</v>
       </c>
       <c r="B2" t="s">
-        <v>798</v>
+        <v>795</v>
       </c>
       <c r="C2" t="s">
-        <v>799</v>
+        <v>796</v>
       </c>
       <c r="D2">
         <v>0</v>

</xml_diff>

<commit_message>
Fix: Use schedule setting for PV.
</commit_message>
<xml_diff>
--- a/rack_v2.0/PLC/type_A/data/global_variable_template.xlsx
+++ b/rack_v2.0/PLC/type_A/data/global_variable_template.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1597" uniqueCount="837">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1599" uniqueCount="837">
   <si>
     <t>[3(FALSE)]</t>
   </si>
@@ -1869,9 +1869,6 @@
     <t>FEEDBACK_shelf_numtray</t>
   </si>
   <si>
-    <t>Pump operation mode (0 - auto, 1 - flowrate, 2 - RPM)</t>
-  </si>
-  <si>
     <t>CTRL_pump_on</t>
   </si>
   <si>
@@ -2548,6 +2545,9 @@
   </si>
   <si>
     <t>D4725</t>
+  </si>
+  <si>
+    <t>Pump operation mode (1 - auto, 2 - flowrate, 3 - RPM)</t>
   </si>
 </sst>
 </file>
@@ -3208,7 +3208,7 @@
         <v>133</v>
       </c>
       <c r="G16" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
@@ -3338,10 +3338,10 @@
         <v>12</v>
       </c>
       <c r="D24" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="E24" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="G24" t="s">
         <v>280</v>
@@ -3355,10 +3355,10 @@
         <v>12</v>
       </c>
       <c r="D25" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="E25" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="G25" t="s">
         <v>281</v>
@@ -3372,10 +3372,10 @@
         <v>12</v>
       </c>
       <c r="D26" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="E26" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="G26" t="s">
         <v>282</v>
@@ -3389,10 +3389,10 @@
         <v>12</v>
       </c>
       <c r="D27" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="E27" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="G27" t="s">
         <v>283</v>
@@ -3420,10 +3420,10 @@
         <v>12</v>
       </c>
       <c r="D29" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="E29" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="G29" t="s">
         <v>284</v>
@@ -3437,10 +3437,10 @@
         <v>12</v>
       </c>
       <c r="D30" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="E30" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="G30" t="s">
         <v>285</v>
@@ -3984,10 +3984,10 @@
         <v>12</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="E59" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="G59" t="s">
         <v>381</v>
@@ -4001,10 +4001,10 @@
         <v>12</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="E60" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="G60" t="s">
         <v>380</v>
@@ -4078,10 +4078,10 @@
         <v>12</v>
       </c>
       <c r="D64" s="8" t="s">
+        <v>790</v>
+      </c>
+      <c r="E64" t="s">
         <v>791</v>
-      </c>
-      <c r="E64" t="s">
-        <v>792</v>
       </c>
       <c r="F64" t="s">
         <v>133</v>
@@ -4092,194 +4092,194 @@
     </row>
     <row r="65" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="C65">
         <v>12</v>
       </c>
       <c r="D65" s="8" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="E65" s="7" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="G65" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="66" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="C66">
         <v>12</v>
       </c>
       <c r="D66" s="8" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="E66" s="7" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="G66" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="67" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="C67">
         <v>12</v>
       </c>
       <c r="D67" s="8" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="E67" s="7" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="G67" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="68" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="C68">
         <v>12</v>
       </c>
       <c r="D68" s="8" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="E68" s="7" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="G68" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="69" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="C69">
         <v>12</v>
       </c>
       <c r="D69" s="8" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="E69" s="7" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="G69" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="70" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="C70">
         <v>12</v>
       </c>
       <c r="D70" s="8" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="E70" s="7" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="G70" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="71" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="C71">
         <v>12</v>
       </c>
       <c r="D71" s="8" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="E71" s="7" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="G71" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="72" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="C72">
         <v>12</v>
       </c>
       <c r="D72" s="8" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="E72" s="7" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="G72" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
     </row>
     <row r="73" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="C73">
         <v>12</v>
       </c>
       <c r="D73" s="8" t="s">
+        <v>790</v>
+      </c>
+      <c r="E73" s="7" t="s">
         <v>791</v>
       </c>
-      <c r="E73" s="7" t="s">
-        <v>792</v>
-      </c>
       <c r="G73" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="74" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="C74">
         <v>12</v>
       </c>
       <c r="D74" s="8" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="E74" s="7" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="G74" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="75" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="C75">
         <v>12</v>
       </c>
       <c r="D75" s="8" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="E75" s="7" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="G75" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
     <row r="76" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="C76">
         <v>3</v>
@@ -4291,7 +4291,7 @@
         <v>0</v>
       </c>
       <c r="G76" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
   </sheetData>
@@ -5619,7 +5619,7 @@
         <v>133</v>
       </c>
       <c r="G6" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -6041,8 +6041,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G199"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A174" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K200" sqref="K200"/>
+    <sheetView tabSelected="1" topLeftCell="A133" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F151" sqref="F151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6082,7 +6082,7 @@
         <v>476</v>
       </c>
       <c r="B2" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -6096,7 +6096,7 @@
         <v>477</v>
       </c>
       <c r="B3" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
@@ -6110,7 +6110,7 @@
         <v>478</v>
       </c>
       <c r="B4" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="C4" t="s">
         <v>1</v>
@@ -6124,7 +6124,7 @@
         <v>479</v>
       </c>
       <c r="B5" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="C5" t="s">
         <v>1</v>
@@ -6138,7 +6138,7 @@
         <v>480</v>
       </c>
       <c r="B6" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="C6" t="s">
         <v>1</v>
@@ -6152,7 +6152,7 @@
         <v>481</v>
       </c>
       <c r="B7" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="C7" t="s">
         <v>1</v>
@@ -6166,7 +6166,7 @@
         <v>482</v>
       </c>
       <c r="B8" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="C8" t="s">
         <v>1</v>
@@ -6180,7 +6180,7 @@
         <v>483</v>
       </c>
       <c r="B9" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="C9" t="s">
         <v>1</v>
@@ -6194,7 +6194,7 @@
         <v>484</v>
       </c>
       <c r="B10" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="C10" t="s">
         <v>1</v>
@@ -6208,7 +6208,7 @@
         <v>485</v>
       </c>
       <c r="B11" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="C11" t="s">
         <v>1</v>
@@ -6222,7 +6222,7 @@
         <v>486</v>
       </c>
       <c r="B12" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="C12" t="s">
         <v>1</v>
@@ -6236,7 +6236,7 @@
         <v>487</v>
       </c>
       <c r="B13" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="C13" t="s">
         <v>1</v>
@@ -6352,7 +6352,7 @@
         <v>494</v>
       </c>
       <c r="B20" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C20" t="s">
         <v>3</v>
@@ -6369,7 +6369,7 @@
         <v>495</v>
       </c>
       <c r="B21" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="C21" t="s">
         <v>3</v>
@@ -6386,7 +6386,7 @@
         <v>496</v>
       </c>
       <c r="B22" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="C22" t="s">
         <v>3</v>
@@ -6403,7 +6403,7 @@
         <v>497</v>
       </c>
       <c r="B23" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="C23" t="s">
         <v>3</v>
@@ -6420,7 +6420,7 @@
         <v>498</v>
       </c>
       <c r="B24" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="C24" t="s">
         <v>3</v>
@@ -6437,7 +6437,7 @@
         <v>499</v>
       </c>
       <c r="B25" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="C25" t="s">
         <v>3</v>
@@ -6614,7 +6614,7 @@
         <v>411</v>
       </c>
       <c r="B34" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C34" t="s">
         <v>3</v>
@@ -6626,7 +6626,7 @@
         <v>133</v>
       </c>
       <c r="F34" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -6634,7 +6634,7 @@
         <v>412</v>
       </c>
       <c r="B35" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="C35" t="s">
         <v>3</v>
@@ -6646,7 +6646,7 @@
         <v>133</v>
       </c>
       <c r="F35" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -6943,7 +6943,7 @@
         <v>131</v>
       </c>
       <c r="F50" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -6960,7 +6960,7 @@
         <v>131</v>
       </c>
       <c r="F51" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -6977,7 +6977,7 @@
         <v>131</v>
       </c>
       <c r="F52" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -6994,12 +6994,12 @@
         <v>131</v>
       </c>
       <c r="F53" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="B54" t="s">
         <v>466</v>
@@ -7011,12 +7011,12 @@
         <v>0</v>
       </c>
       <c r="F54" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="B55" t="s">
         <v>467</v>
@@ -7028,7 +7028,7 @@
         <v>0</v>
       </c>
       <c r="F55" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -7045,7 +7045,7 @@
         <v>131</v>
       </c>
       <c r="F56" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
@@ -7062,7 +7062,7 @@
         <v>131</v>
       </c>
       <c r="F57" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -7206,7 +7206,7 @@
         <v>458</v>
       </c>
       <c r="B66" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="C66" t="s">
         <v>3</v>
@@ -7223,7 +7223,7 @@
         <v>459</v>
       </c>
       <c r="B67" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="C67" t="s">
         <v>3</v>
@@ -7240,7 +7240,7 @@
         <v>238</v>
       </c>
       <c r="B68" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="C68" t="s">
         <v>3</v>
@@ -7257,7 +7257,7 @@
         <v>239</v>
       </c>
       <c r="B69" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="C69" t="s">
         <v>3</v>
@@ -7274,7 +7274,7 @@
         <v>240</v>
       </c>
       <c r="B70" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="C70" t="s">
         <v>3</v>
@@ -7291,7 +7291,7 @@
         <v>241</v>
       </c>
       <c r="B71" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="C71" t="s">
         <v>3</v>
@@ -7308,7 +7308,7 @@
         <v>242</v>
       </c>
       <c r="B72" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="C72" t="s">
         <v>3</v>
@@ -7325,7 +7325,7 @@
         <v>243</v>
       </c>
       <c r="B73" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="C73" t="s">
         <v>3</v>
@@ -7342,7 +7342,7 @@
         <v>244</v>
       </c>
       <c r="B74" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="C74" t="s">
         <v>3</v>
@@ -7359,7 +7359,7 @@
         <v>245</v>
       </c>
       <c r="B75" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="C75" t="s">
         <v>3</v>
@@ -7376,7 +7376,7 @@
         <v>246</v>
       </c>
       <c r="B76" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="C76" t="s">
         <v>3</v>
@@ -7393,7 +7393,7 @@
         <v>247</v>
       </c>
       <c r="B77" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="C77" t="s">
         <v>3</v>
@@ -7410,7 +7410,7 @@
         <v>474</v>
       </c>
       <c r="B78" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="C78" t="s">
         <v>3</v>
@@ -7427,7 +7427,7 @@
         <v>475</v>
       </c>
       <c r="B79" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="C79" t="s">
         <v>3</v>
@@ -7444,7 +7444,7 @@
         <v>228</v>
       </c>
       <c r="B80" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="C80" t="s">
         <v>1</v>
@@ -7453,7 +7453,7 @@
         <v>-1</v>
       </c>
       <c r="F80" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
@@ -7461,7 +7461,7 @@
         <v>229</v>
       </c>
       <c r="B81" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="C81" t="s">
         <v>1</v>
@@ -7470,7 +7470,7 @@
         <v>-1</v>
       </c>
       <c r="F81" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
@@ -7478,7 +7478,7 @@
         <v>230</v>
       </c>
       <c r="B82" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="C82" t="s">
         <v>1</v>
@@ -7495,7 +7495,7 @@
         <v>231</v>
       </c>
       <c r="B83" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="C83" t="s">
         <v>1</v>
@@ -7512,7 +7512,7 @@
         <v>232</v>
       </c>
       <c r="B84" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="C84" t="s">
         <v>1</v>
@@ -7529,7 +7529,7 @@
         <v>233</v>
       </c>
       <c r="B85" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="C85" t="s">
         <v>1</v>
@@ -7546,7 +7546,7 @@
         <v>234</v>
       </c>
       <c r="B86" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="C86" t="s">
         <v>1</v>
@@ -7563,7 +7563,7 @@
         <v>235</v>
       </c>
       <c r="B87" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="C87" t="s">
         <v>1</v>
@@ -7580,7 +7580,7 @@
         <v>236</v>
       </c>
       <c r="B88" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="C88" t="s">
         <v>1</v>
@@ -7597,7 +7597,7 @@
         <v>237</v>
       </c>
       <c r="B89" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="C89" t="s">
         <v>1</v>
@@ -7614,7 +7614,7 @@
         <v>502</v>
       </c>
       <c r="B90" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="C90" t="s">
         <v>1</v>
@@ -7631,7 +7631,7 @@
         <v>503</v>
       </c>
       <c r="B91" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="C91" t="s">
         <v>1</v>
@@ -7648,7 +7648,7 @@
         <v>506</v>
       </c>
       <c r="B92" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="C92" t="s">
         <v>1</v>
@@ -7665,7 +7665,7 @@
         <v>507</v>
       </c>
       <c r="B93" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="C93" t="s">
         <v>1</v>
@@ -7682,7 +7682,7 @@
         <v>508</v>
       </c>
       <c r="B94" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="C94" t="s">
         <v>1</v>
@@ -7699,7 +7699,7 @@
         <v>509</v>
       </c>
       <c r="B95" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="C95" t="s">
         <v>1</v>
@@ -8110,10 +8110,10 @@
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B119" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="C119" t="s">
         <v>316</v>
@@ -8122,15 +8122,15 @@
         <v>-1</v>
       </c>
       <c r="F119" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="B120" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="C120" t="s">
         <v>316</v>
@@ -8139,15 +8139,15 @@
         <v>-1</v>
       </c>
       <c r="F120" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="B121" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="C121" t="s">
         <v>316</v>
@@ -8156,15 +8156,15 @@
         <v>-1</v>
       </c>
       <c r="F121" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="B122" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="C122" t="s">
         <v>316</v>
@@ -8173,7 +8173,7 @@
         <v>-1</v>
       </c>
       <c r="F122" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
@@ -8229,10 +8229,10 @@
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
+        <v>652</v>
+      </c>
+      <c r="B126" t="s">
         <v>653</v>
-      </c>
-      <c r="B126" t="s">
-        <v>654</v>
       </c>
       <c r="C126" t="s">
         <v>1</v>
@@ -8244,15 +8244,15 @@
         <v>133</v>
       </c>
       <c r="F126" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
+        <v>654</v>
+      </c>
+      <c r="B127" t="s">
         <v>655</v>
-      </c>
-      <c r="B127" t="s">
-        <v>656</v>
       </c>
       <c r="C127" t="s">
         <v>1</v>
@@ -8264,15 +8264,15 @@
         <v>133</v>
       </c>
       <c r="F127" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
+        <v>657</v>
+      </c>
+      <c r="B128" t="s">
         <v>658</v>
-      </c>
-      <c r="B128" t="s">
-        <v>659</v>
       </c>
       <c r="C128" t="s">
         <v>1</v>
@@ -8284,15 +8284,15 @@
         <v>133</v>
       </c>
       <c r="F128" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
+        <v>796</v>
+      </c>
+      <c r="B129" t="s">
         <v>797</v>
-      </c>
-      <c r="B129" t="s">
-        <v>798</v>
       </c>
       <c r="C129" t="s">
         <v>1</v>
@@ -8304,35 +8304,35 @@
         <v>133</v>
       </c>
       <c r="F129" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
+        <v>662</v>
+      </c>
+      <c r="B130" t="s">
         <v>663</v>
       </c>
-      <c r="B130" t="s">
+      <c r="C130" t="s">
         <v>664</v>
       </c>
-      <c r="C130" t="s">
+      <c r="D130" t="s">
         <v>665</v>
       </c>
-      <c r="D130" t="s">
+      <c r="E130" t="s">
+        <v>133</v>
+      </c>
+      <c r="F130" t="s">
         <v>666</v>
-      </c>
-      <c r="E130" t="s">
-        <v>133</v>
-      </c>
-      <c r="F130" t="s">
-        <v>667</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
+        <v>745</v>
+      </c>
+      <c r="B131" t="s">
         <v>746</v>
-      </c>
-      <c r="B131" t="s">
-        <v>747</v>
       </c>
       <c r="C131" t="s">
         <v>3</v>
@@ -8344,15 +8344,15 @@
         <v>133</v>
       </c>
       <c r="F131" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
+        <v>757</v>
+      </c>
+      <c r="B132" t="s">
         <v>758</v>
-      </c>
-      <c r="B132" t="s">
-        <v>759</v>
       </c>
       <c r="C132" t="s">
         <v>3</v>
@@ -8364,7 +8364,7 @@
         <v>133</v>
       </c>
       <c r="F132" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
@@ -8375,10 +8375,10 @@
         <v>332</v>
       </c>
       <c r="C133" s="8" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="D133" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="E133" t="s">
         <v>133</v>
@@ -8395,10 +8395,10 @@
         <v>533</v>
       </c>
       <c r="C134" s="8" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="D134" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="E134" t="s">
         <v>133</v>
@@ -8415,10 +8415,10 @@
         <v>534</v>
       </c>
       <c r="C135" s="8" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="D135" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="F135" t="s">
         <v>540</v>
@@ -8449,10 +8449,10 @@
         <v>539</v>
       </c>
       <c r="C137" s="8" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="D137" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="F137" t="s">
         <v>545</v>
@@ -8466,10 +8466,10 @@
         <v>542</v>
       </c>
       <c r="C138" t="s">
+        <v>790</v>
+      </c>
+      <c r="D138" t="s">
         <v>791</v>
-      </c>
-      <c r="D138" t="s">
-        <v>792</v>
       </c>
       <c r="F138" t="s">
         <v>543</v>
@@ -8477,22 +8477,22 @@
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
+        <v>772</v>
+      </c>
+      <c r="B139" t="s">
         <v>773</v>
       </c>
-      <c r="B139" t="s">
+      <c r="C139" s="8" t="s">
+        <v>789</v>
+      </c>
+      <c r="D139" t="s">
+        <v>787</v>
+      </c>
+      <c r="E139" t="s">
+        <v>133</v>
+      </c>
+      <c r="F139" t="s">
         <v>774</v>
-      </c>
-      <c r="C139" s="8" t="s">
-        <v>790</v>
-      </c>
-      <c r="D139" t="s">
-        <v>788</v>
-      </c>
-      <c r="E139" t="s">
-        <v>133</v>
-      </c>
-      <c r="F139" t="s">
-        <v>775</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.25">
@@ -8597,10 +8597,10 @@
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
+        <v>670</v>
+      </c>
+      <c r="B145" t="s">
         <v>671</v>
-      </c>
-      <c r="B145" t="s">
-        <v>672</v>
       </c>
       <c r="C145" t="s">
         <v>2</v>
@@ -8612,7 +8612,7 @@
         <v>133</v>
       </c>
       <c r="F145" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.25">
@@ -8657,10 +8657,10 @@
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="B148" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="C148" s="8" t="s">
         <v>11</v>
@@ -8672,7 +8672,7 @@
         <v>133</v>
       </c>
       <c r="F148" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.25">
@@ -8683,10 +8683,10 @@
         <v>555</v>
       </c>
       <c r="C149" t="s">
+        <v>790</v>
+      </c>
+      <c r="D149" t="s">
         <v>791</v>
-      </c>
-      <c r="D149" t="s">
-        <v>792</v>
       </c>
       <c r="F149" t="s">
         <v>560</v>
@@ -8700,10 +8700,10 @@
         <v>557</v>
       </c>
       <c r="C150" s="8" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="D150" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="F150" t="s">
         <v>544</v>
@@ -8726,7 +8726,7 @@
         <v>133</v>
       </c>
       <c r="F151" t="s">
-        <v>610</v>
+        <v>836</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">
@@ -8782,6 +8782,9 @@
       <c r="D154" t="s">
         <v>0</v>
       </c>
+      <c r="E154" t="s">
+        <v>133</v>
+      </c>
       <c r="F154" t="s">
         <v>562</v>
       </c>
@@ -8799,6 +8802,9 @@
       <c r="D155" t="s">
         <v>0</v>
       </c>
+      <c r="E155" t="s">
+        <v>133</v>
+      </c>
       <c r="F155" t="s">
         <v>563</v>
       </c>
@@ -8811,10 +8817,10 @@
         <v>573</v>
       </c>
       <c r="C156" s="8" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="D156" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="F156" t="s">
         <v>212</v>
@@ -8825,13 +8831,13 @@
         <v>576</v>
       </c>
       <c r="B157" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="C157" s="8" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="D157" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="F157" t="s">
         <v>211</v>
@@ -8842,13 +8848,13 @@
         <v>577</v>
       </c>
       <c r="B158" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="C158" s="8" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="D158" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="F158" t="s">
         <v>213</v>
@@ -8859,13 +8865,13 @@
         <v>578</v>
       </c>
       <c r="B159" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="C159" s="8" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="D159" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="F159" t="s">
         <v>214</v>
@@ -8876,13 +8882,13 @@
         <v>579</v>
       </c>
       <c r="B160" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="C160" s="8" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="D160" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="F160" t="s">
         <v>522</v>
@@ -8893,13 +8899,13 @@
         <v>580</v>
       </c>
       <c r="B161" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="C161" s="8" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="D161" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="F161" t="s">
         <v>523</v>
@@ -8907,104 +8913,104 @@
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="B162" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="C162" s="8" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="D162" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="F162" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="B163" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="C163" s="8" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="D163" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="F163" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="B164" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="C164" s="8" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="D164" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="F164" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="B165" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="C165" s="8" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="D165" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="F165" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="B166" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="C166" s="8" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="D166" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="F166" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B167" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="C167" s="8" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="D167" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="F167" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.25">
@@ -9012,13 +9018,13 @@
         <v>581</v>
       </c>
       <c r="B168" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="C168" s="8" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="D168" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="E168" t="s">
         <v>133</v>
@@ -9032,13 +9038,13 @@
         <v>582</v>
       </c>
       <c r="B169" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="C169" s="8" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="D169" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="E169" t="s">
         <v>133</v>
@@ -9052,13 +9058,13 @@
         <v>583</v>
       </c>
       <c r="B170" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="C170" s="8" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="D170" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="E170" t="s">
         <v>133</v>
@@ -9072,7 +9078,7 @@
         <v>590</v>
       </c>
       <c r="B171" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="C171" s="8" t="s">
         <v>11</v>
@@ -9089,7 +9095,7 @@
         <v>591</v>
       </c>
       <c r="B172" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="C172" s="8" t="s">
         <v>11</v>
@@ -9106,7 +9112,7 @@
         <v>595</v>
       </c>
       <c r="B173" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="C173" s="8" t="s">
         <v>11</v>
@@ -9123,7 +9129,7 @@
         <v>597</v>
       </c>
       <c r="B174" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="C174" s="8" t="s">
         <v>2</v>
@@ -9140,7 +9146,7 @@
         <v>598</v>
       </c>
       <c r="B175" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="C175" s="8" t="s">
         <v>11</v>
@@ -9154,10 +9160,10 @@
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="B176" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="C176" s="8" t="s">
         <v>2</v>
@@ -9169,35 +9175,35 @@
         <v>133</v>
       </c>
       <c r="F176" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
+        <v>612</v>
+      </c>
+      <c r="B177" t="s">
+        <v>646</v>
+      </c>
+      <c r="C177" s="8" t="s">
+        <v>792</v>
+      </c>
+      <c r="D177" s="7" t="s">
+        <v>793</v>
+      </c>
+      <c r="E177" t="s">
+        <v>133</v>
+      </c>
+      <c r="F177" t="s">
         <v>613</v>
-      </c>
-      <c r="B177" t="s">
-        <v>647</v>
-      </c>
-      <c r="C177" s="8" t="s">
-        <v>793</v>
-      </c>
-      <c r="D177" s="7" t="s">
-        <v>794</v>
-      </c>
-      <c r="E177" t="s">
-        <v>133</v>
-      </c>
-      <c r="F177" t="s">
-        <v>614</v>
       </c>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
+        <v>649</v>
+      </c>
+      <c r="B178" t="s">
         <v>650</v>
-      </c>
-      <c r="B178" t="s">
-        <v>651</v>
       </c>
       <c r="C178" s="8" t="s">
         <v>11</v>
@@ -9209,215 +9215,215 @@
         <v>133</v>
       </c>
       <c r="F178" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
+        <v>659</v>
+      </c>
+      <c r="B179" t="s">
         <v>660</v>
       </c>
-      <c r="B179" t="s">
+      <c r="C179" s="8" t="s">
+        <v>790</v>
+      </c>
+      <c r="D179" s="7" t="s">
+        <v>791</v>
+      </c>
+      <c r="E179" t="s">
+        <v>133</v>
+      </c>
+      <c r="F179" t="s">
         <v>661</v>
-      </c>
-      <c r="C179" s="8" t="s">
-        <v>791</v>
-      </c>
-      <c r="D179" s="7" t="s">
-        <v>792</v>
-      </c>
-      <c r="E179" t="s">
-        <v>133</v>
-      </c>
-      <c r="F179" t="s">
-        <v>662</v>
       </c>
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="B180" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="C180" s="8" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="D180" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="E180" t="s">
         <v>133</v>
       </c>
       <c r="F180" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="B181" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="C181" s="8" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="D181" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="E181" t="s">
         <v>133</v>
       </c>
       <c r="F181" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="B182" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="C182" s="8" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="D182" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="E182" t="s">
         <v>133</v>
       </c>
       <c r="F182" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="B183" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="C183" s="8" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="D183" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="E183" t="s">
         <v>133</v>
       </c>
       <c r="F183" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="B184" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="C184" s="8" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="D184" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="E184" t="s">
         <v>133</v>
       </c>
       <c r="F184" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="B185" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="C185" s="8" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="D185" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="E185" t="s">
         <v>133</v>
       </c>
       <c r="F185" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="B186" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="C186" s="8" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="D186" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="E186" t="s">
         <v>133</v>
       </c>
       <c r="F186" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="B187" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="C187" s="8" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="D187" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="E187" t="s">
         <v>133</v>
       </c>
       <c r="F187" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
+        <v>698</v>
+      </c>
+      <c r="B188" t="s">
         <v>699</v>
       </c>
-      <c r="B188" t="s">
-        <v>700</v>
-      </c>
       <c r="C188" s="8" t="s">
+        <v>790</v>
+      </c>
+      <c r="D188" s="7" t="s">
         <v>791</v>
       </c>
-      <c r="D188" s="7" t="s">
-        <v>792</v>
-      </c>
       <c r="E188" t="s">
         <v>133</v>
       </c>
       <c r="F188" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
+        <v>751</v>
+      </c>
+      <c r="B189" t="s">
         <v>752</v>
-      </c>
-      <c r="B189" t="s">
-        <v>753</v>
       </c>
       <c r="C189" s="8" t="s">
         <v>514</v>
@@ -9429,35 +9435,35 @@
         <v>133</v>
       </c>
       <c r="F189" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
+        <v>754</v>
+      </c>
+      <c r="B190" t="s">
         <v>755</v>
       </c>
-      <c r="B190" t="s">
+      <c r="C190" s="8" t="s">
+        <v>789</v>
+      </c>
+      <c r="D190" s="7" t="s">
+        <v>787</v>
+      </c>
+      <c r="E190" t="s">
+        <v>133</v>
+      </c>
+      <c r="F190" t="s">
         <v>756</v>
-      </c>
-      <c r="C190" s="8" t="s">
-        <v>790</v>
-      </c>
-      <c r="D190" s="7" t="s">
-        <v>788</v>
-      </c>
-      <c r="E190" t="s">
-        <v>133</v>
-      </c>
-      <c r="F190" t="s">
-        <v>757</v>
       </c>
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
+        <v>769</v>
+      </c>
+      <c r="B191" t="s">
         <v>770</v>
-      </c>
-      <c r="B191" t="s">
-        <v>771</v>
       </c>
       <c r="C191" s="8" t="s">
         <v>2</v>
@@ -9469,55 +9475,55 @@
         <v>133</v>
       </c>
       <c r="F191" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
+        <v>775</v>
+      </c>
+      <c r="B192" t="s">
         <v>776</v>
       </c>
-      <c r="B192" t="s">
-        <v>777</v>
-      </c>
       <c r="C192" s="8" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="D192" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="E192" t="s">
         <v>133</v>
       </c>
       <c r="F192" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
+        <v>777</v>
+      </c>
+      <c r="B193" t="s">
         <v>778</v>
       </c>
-      <c r="B193" t="s">
-        <v>779</v>
-      </c>
       <c r="C193" s="8" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="D193" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="E193" t="s">
         <v>133</v>
       </c>
       <c r="F193" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="B194" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="C194" s="8" t="s">
         <v>11</v>
@@ -9529,35 +9535,35 @@
         <v>133</v>
       </c>
       <c r="F194" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="B195" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="C195" s="8" t="s">
         <v>11</v>
       </c>
       <c r="D195" s="7" t="s">
+        <v>832</v>
+      </c>
+      <c r="E195" t="s">
+        <v>133</v>
+      </c>
+      <c r="F195" t="s">
         <v>833</v>
-      </c>
-      <c r="E195" t="s">
-        <v>133</v>
-      </c>
-      <c r="F195" t="s">
-        <v>834</v>
       </c>
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="B196" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="C196" s="8" t="s">
         <v>316</v>
@@ -9569,15 +9575,15 @@
         <v>133</v>
       </c>
       <c r="F196" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="B197" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="C197" s="8" t="s">
         <v>316</v>
@@ -9589,15 +9595,15 @@
         <v>133</v>
       </c>
       <c r="F197" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="B198" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="C198" s="8" t="s">
         <v>316</v>
@@ -9609,15 +9615,15 @@
         <v>133</v>
       </c>
       <c r="F198" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="B199" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="C199" s="8" t="s">
         <v>316</v>
@@ -9629,7 +9635,7 @@
         <v>133</v>
       </c>
       <c r="F199" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
     </row>
   </sheetData>
@@ -9679,10 +9685,10 @@
         <v>1000</v>
       </c>
       <c r="B2" t="s">
+        <v>794</v>
+      </c>
+      <c r="C2" t="s">
         <v>795</v>
-      </c>
-      <c r="C2" t="s">
-        <v>796</v>
       </c>
       <c r="D2">
         <v>0</v>

</xml_diff>

<commit_message>
Restore pump speed limiter Add error recovery after 10 mins shutdown
</commit_message>
<xml_diff>
--- a/rack_v2.0/PLC/type_A/data/global_variable_template.xlsx
+++ b/rack_v2.0/PLC/type_A/data/global_variable_template.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\Ellemento\repo\Ellemento_dev\rack_v2.0\PLC\type_A\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\Ellemento\Part 1\repo\Ellemento\rack_v2.0\PLC\type_A\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="14370" windowHeight="10500" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="14370" windowHeight="10500" firstSheet="3" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Constants" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1599" uniqueCount="837">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1610" uniqueCount="842">
   <si>
     <t>[3(FALSE)]</t>
   </si>
@@ -2548,6 +2548,21 @@
   </si>
   <si>
     <t>Pump operation mode (1 - auto, 2 - flowrate, 3 - RPM)</t>
+  </si>
+  <si>
+    <t>pumpRecoverySequenceStarted</t>
+  </si>
+  <si>
+    <t>pumpRecoveryStartTime</t>
+  </si>
+  <si>
+    <t>flag to start recovery</t>
+  </si>
+  <si>
+    <t>REF_pump_error_shutdown_recovery_time_m</t>
+  </si>
+  <si>
+    <t>D4730</t>
   </si>
 </sst>
 </file>
@@ -5486,10 +5501,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H28"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6014,21 +6029,52 @@
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
+        <v>837</v>
+      </c>
+      <c r="C28">
+        <v>3</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E28" t="s">
+        <v>0</v>
+      </c>
+      <c r="G28" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>838</v>
+      </c>
+      <c r="C29">
+        <v>3</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E29" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
         <v>271</v>
       </c>
-      <c r="C28">
-        <v>3</v>
-      </c>
-      <c r="D28" s="8" t="s">
+      <c r="C30">
+        <v>3</v>
+      </c>
+      <c r="D30" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E28" s="7" t="s">
+      <c r="E30" s="7" t="s">
         <v>398</v>
       </c>
-      <c r="F28" t="s">
-        <v>133</v>
-      </c>
-      <c r="G28" t="s">
+      <c r="F30" t="s">
+        <v>133</v>
+      </c>
+      <c r="G30" t="s">
         <v>260</v>
       </c>
     </row>
@@ -6039,10 +6085,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G199"/>
+  <dimension ref="A1:G200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F151" sqref="F151"/>
+    <sheetView tabSelected="1" topLeftCell="A163" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C194" sqref="C194"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9636,6 +9682,20 @@
       </c>
       <c r="F199" t="s">
         <v>828</v>
+      </c>
+    </row>
+    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
+        <v>840</v>
+      </c>
+      <c r="B200" t="s">
+        <v>841</v>
+      </c>
+      <c r="C200" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D200" s="7" t="s">
+        <v>832</v>
       </c>
     </row>
   </sheetData>

</xml_diff>